<commit_message>
Melhorias no módulo de Simulador
</commit_message>
<xml_diff>
--- a/uploads/modelo.xlsx
+++ b/uploads/modelo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deza_\Documents\server\sustentech\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B89AA9-5861-4362-B30B-98610A2DEA42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B94F7EBA-9896-4283-8595-9E57FDAEFF79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{CD22A53C-7A42-42CD-B37C-4F19A518B943}"/>
   </bookViews>
@@ -38,16 +38,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>CONSUMO</t>
-  </si>
-  <si>
     <t>DATA DE REFERÊNCIA</t>
   </si>
   <si>
-    <t>VALOR PAGO</t>
+    <t>(R$) VALOR PAGO</t>
   </si>
   <si>
-    <t>REUTILIZADO</t>
+    <t>REUTILIZADO (m³)</t>
+  </si>
+  <si>
+    <t>CONSUMO (m³)</t>
   </si>
 </sst>
 </file>
@@ -460,34 +460,34 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>36526</v>
+        <v>36161</v>
       </c>
       <c r="B2" s="1">
         <v>100</v>

</xml_diff>